<commit_message>
insurance policy test fixes
</commit_message>
<xml_diff>
--- a/testing/testSuite/src/main/resources/TestInsurancePolicyStandardisation/testDayOnDayProcessing/SeedData-Day3.xlsx
+++ b/testing/testSuite/src/main/resources/TestInsurancePolicyStandardisation/testDayOnDayProcessing/SeedData-Day3.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA86788-EC81-48DF-804F-8BB592744466}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1575" yWindow="0" windowWidth="20025" windowHeight="10320" tabRatio="725" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="725" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="feed" sheetId="1" r:id="rId1"/>
@@ -17,17 +18,25 @@
     <sheet name="insurance_policy_tax_jurisd" sheetId="14" r:id="rId8"/>
     <sheet name="fr_general_codes" sheetId="18" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="206">
   <si>
     <t>N</t>
   </si>
@@ -104,24 +113,9 @@
     <t>A</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>USD</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>9</t>
   </si>
   <si>
@@ -248,36 +242,6 @@
     <t>J</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>2010</t>
-  </si>
-  <si>
     <t>ASSUMED</t>
   </si>
   <si>
@@ -287,78 +251,9 @@
     <t>PP</t>
   </si>
   <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>102</t>
-  </si>
-  <si>
-    <t>103</t>
-  </si>
-  <si>
-    <t>104</t>
-  </si>
-  <si>
-    <t>105</t>
-  </si>
-  <si>
-    <t>106</t>
-  </si>
-  <si>
-    <t>107</t>
-  </si>
-  <si>
-    <t>108</t>
-  </si>
-  <si>
-    <t>109</t>
-  </si>
-  <si>
-    <t>201</t>
-  </si>
-  <si>
-    <t>202</t>
-  </si>
-  <si>
-    <t>203</t>
-  </si>
-  <si>
-    <t>204</t>
-  </si>
-  <si>
-    <t>205</t>
-  </si>
-  <si>
-    <t>206</t>
-  </si>
-  <si>
-    <t>207</t>
-  </si>
-  <si>
-    <t>208</t>
-  </si>
-  <si>
-    <t>209</t>
-  </si>
-  <si>
-    <t>210</t>
-  </si>
-  <si>
     <t>CEDED</t>
   </si>
   <si>
-    <t>2011</t>
-  </si>
-  <si>
-    <t>2012</t>
-  </si>
-  <si>
-    <t>211</t>
-  </si>
-  <si>
-    <t>212</t>
-  </si>
-  <si>
     <t>US</t>
   </si>
   <si>
@@ -554,9 +449,6 @@
     <t>Parent LE109</t>
   </si>
   <si>
-    <t>110</t>
-  </si>
-  <si>
     <t>LE110</t>
   </si>
   <si>
@@ -708,12 +600,6 @@
   </si>
   <si>
     <t>586F8FB9FC7121F2E053D3830A0AC0F3</t>
-  </si>
-  <si>
-    <t>2013</t>
-  </si>
-  <si>
-    <t>2014</t>
   </si>
   <si>
     <t>POLICY_NM</t>
@@ -773,7 +659,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -824,7 +710,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -836,9 +722,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -866,6 +750,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1180,7 +1070,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1190,111 +1080,111 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="19.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="1" width="34.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="8" t="s">
+    <row r="3" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="14">
+      <c r="A4" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="12">
         <v>42916</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="13">
         <v>43164.654861111114</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="12" t="s">
-        <v>226</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="C5" s="14">
+      <c r="A5" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="C5" s="12">
         <v>42916</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="F5" s="15">
+      <c r="E5" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="F5" s="13">
         <v>43164.655555555553</v>
       </c>
     </row>
@@ -1305,7 +1195,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1315,150 +1205,150 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="11"/>
+    <col min="1" max="1" width="34.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="A3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="B4" s="9" t="s">
+      <c r="A4" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="12">
+      <c r="C4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A5" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="B5" s="9" t="s">
+      <c r="A5" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="12">
+      <c r="C5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="B6" s="9" t="s">
+      <c r="A6" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="12">
+      <c r="C6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A7" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="B7" s="9" t="s">
+      <c r="A7" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="12">
+      <c r="C7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="B8" s="9" t="s">
+      <c r="A8" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="12">
+      <c r="C8" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A9" s="12" t="s">
-        <v>226</v>
-      </c>
-      <c r="B9" s="9" t="s">
+      <c r="A9" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="D9" s="12">
+      <c r="C9" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="D9" s="10">
         <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A10" s="12" t="s">
-        <v>226</v>
-      </c>
-      <c r="B10" s="9" t="s">
+      <c r="A10" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>216</v>
-      </c>
-      <c r="D10" s="12">
+      <c r="C10" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="D10" s="10">
         <v>0</v>
       </c>
     </row>
@@ -1468,17 +1358,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
+      <selection pane="bottomLeft" activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
@@ -1491,39 +1381,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>51</v>
+      <c r="A1" s="14" t="s">
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>206</v>
+        <v>167</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>207</v>
+        <v>168</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>208</v>
+        <v>169</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>209</v>
+        <v>170</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>211</v>
+        <v>172</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>212</v>
+        <v>173</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>246</v>
+        <v>205</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="14" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1555,7 +1445,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1587,789 +1477,789 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>27</v>
+      <c r="A4" s="15">
+        <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>174</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="15">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>174</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="15">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" t="s">
         <v>115</v>
       </c>
-      <c r="C4" t="s">
-        <v>151</v>
-      </c>
-      <c r="D4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" t="s">
-        <v>213</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H4" t="s">
-        <v>0</v>
-      </c>
-      <c r="I4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>174</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" t="s">
         <v>116</v>
       </c>
-      <c r="C5" t="s">
-        <v>152</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" t="s">
-        <v>213</v>
-      </c>
-      <c r="F5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" t="s">
-        <v>0</v>
-      </c>
-      <c r="H5" t="s">
-        <v>0</v>
-      </c>
-      <c r="I5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>174</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" t="s">
         <v>117</v>
       </c>
-      <c r="C6" t="s">
-        <v>153</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" t="s">
-        <v>213</v>
-      </c>
-      <c r="F6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" t="s">
-        <v>0</v>
-      </c>
-      <c r="H6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>174</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="15">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" t="s">
         <v>118</v>
       </c>
-      <c r="C7" t="s">
-        <v>154</v>
-      </c>
-      <c r="D7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" t="s">
-        <v>213</v>
-      </c>
-      <c r="F7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H7" t="s">
-        <v>0</v>
-      </c>
-      <c r="I7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="D9" t="s">
         <v>25</v>
       </c>
-      <c r="B8" t="s">
+      <c r="E9" t="s">
+        <v>174</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="15">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" t="s">
         <v>119</v>
       </c>
-      <c r="C8" t="s">
-        <v>155</v>
-      </c>
-      <c r="D8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" t="s">
-        <v>213</v>
-      </c>
-      <c r="F8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H8" t="s">
-        <v>0</v>
-      </c>
-      <c r="I8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" t="s">
+        <v>174</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" t="s">
         <v>120</v>
       </c>
-      <c r="C9" t="s">
-        <v>156</v>
-      </c>
-      <c r="D9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" t="s">
-        <v>213</v>
-      </c>
-      <c r="F9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" t="s">
-        <v>0</v>
-      </c>
-      <c r="H9" t="s">
-        <v>0</v>
-      </c>
-      <c r="I9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" t="s">
+        <v>174</v>
+      </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" t="s">
         <v>121</v>
       </c>
-      <c r="C10" t="s">
-        <v>157</v>
-      </c>
-      <c r="D10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" t="s">
-        <v>213</v>
-      </c>
-      <c r="F10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H10" t="s">
-        <v>0</v>
-      </c>
-      <c r="I10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" t="s">
+        <v>174</v>
+      </c>
+      <c r="F12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" t="s">
         <v>122</v>
       </c>
-      <c r="C11" t="s">
-        <v>158</v>
-      </c>
-      <c r="D11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" t="s">
-        <v>213</v>
-      </c>
-      <c r="F11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" t="s">
-        <v>0</v>
-      </c>
-      <c r="H11" t="s">
-        <v>0</v>
-      </c>
-      <c r="I11" t="s">
-        <v>23</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" t="s">
+        <v>174</v>
+      </c>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" t="s">
         <v>123</v>
       </c>
-      <c r="C12" t="s">
-        <v>159</v>
-      </c>
-      <c r="D12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" t="s">
-        <v>213</v>
-      </c>
-      <c r="F12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" t="s">
-        <v>0</v>
-      </c>
-      <c r="H12" t="s">
-        <v>0</v>
-      </c>
-      <c r="I12" t="s">
-        <v>23</v>
-      </c>
-      <c r="J12" s="12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" t="s">
+        <v>178</v>
+      </c>
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" t="s">
         <v>124</v>
       </c>
-      <c r="C13" t="s">
-        <v>160</v>
-      </c>
-      <c r="D13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" t="s">
-        <v>213</v>
-      </c>
-      <c r="F13" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" t="s">
-        <v>0</v>
-      </c>
-      <c r="H13" t="s">
-        <v>0</v>
-      </c>
-      <c r="I13" t="s">
-        <v>23</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" t="s">
+        <v>178</v>
+      </c>
+      <c r="F15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" t="s">
         <v>125</v>
       </c>
-      <c r="C14" t="s">
-        <v>161</v>
-      </c>
-      <c r="D14" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" t="s">
-        <v>217</v>
-      </c>
-      <c r="F14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" t="s">
-        <v>0</v>
-      </c>
-      <c r="H14" t="s">
-        <v>0</v>
-      </c>
-      <c r="I14" t="s">
-        <v>23</v>
-      </c>
-      <c r="J14" s="12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" t="s">
+        <v>178</v>
+      </c>
+      <c r="F16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>23</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="15">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" t="s">
         <v>126</v>
       </c>
-      <c r="C15" t="s">
-        <v>162</v>
-      </c>
-      <c r="D15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" t="s">
-        <v>217</v>
-      </c>
-      <c r="F15" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" t="s">
-        <v>0</v>
-      </c>
-      <c r="H15" t="s">
-        <v>0</v>
-      </c>
-      <c r="I15" t="s">
-        <v>23</v>
-      </c>
-      <c r="J15" s="12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="D17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" t="s">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="15">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" t="s">
         <v>127</v>
       </c>
-      <c r="C16" t="s">
-        <v>163</v>
-      </c>
-      <c r="D16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" t="s">
-        <v>217</v>
-      </c>
-      <c r="F16" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" t="s">
-        <v>0</v>
-      </c>
-      <c r="H16" t="s">
-        <v>0</v>
-      </c>
-      <c r="I16" t="s">
-        <v>23</v>
-      </c>
-      <c r="J16" s="12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="D18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" t="s">
+        <v>178</v>
+      </c>
+      <c r="F18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18" t="s">
+        <v>0</v>
+      </c>
+      <c r="I18" t="s">
+        <v>23</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="16">
+        <v>101</v>
+      </c>
+      <c r="B19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" t="s">
         <v>128</v>
       </c>
-      <c r="C17" t="s">
-        <v>164</v>
-      </c>
-      <c r="D17" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" t="s">
-        <v>217</v>
-      </c>
-      <c r="F17" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" t="s">
-        <v>0</v>
-      </c>
-      <c r="H17" t="s">
-        <v>0</v>
-      </c>
-      <c r="I17" t="s">
-        <v>23</v>
-      </c>
-      <c r="J17" s="12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" t="s">
+        <v>174</v>
+      </c>
+      <c r="F19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H19" t="s">
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="16">
+        <v>102</v>
+      </c>
+      <c r="B20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" t="s">
         <v>129</v>
       </c>
-      <c r="C18" t="s">
-        <v>165</v>
-      </c>
-      <c r="D18" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" t="s">
-        <v>217</v>
-      </c>
-      <c r="F18" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18" t="s">
-        <v>0</v>
-      </c>
-      <c r="H18" t="s">
-        <v>0</v>
-      </c>
-      <c r="I18" t="s">
-        <v>23</v>
-      </c>
-      <c r="J18" s="12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="D20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" t="s">
+        <v>174</v>
+      </c>
+      <c r="F20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" t="s">
+        <v>0</v>
+      </c>
+      <c r="H20" t="s">
+        <v>0</v>
+      </c>
+      <c r="I20" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="16">
+        <v>103</v>
+      </c>
+      <c r="B21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" t="s">
         <v>130</v>
       </c>
-      <c r="C19" t="s">
-        <v>166</v>
-      </c>
-      <c r="D19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" t="s">
-        <v>213</v>
-      </c>
-      <c r="F19" t="s">
-        <v>23</v>
-      </c>
-      <c r="G19" t="s">
-        <v>0</v>
-      </c>
-      <c r="H19" t="s">
-        <v>0</v>
-      </c>
-      <c r="I19" t="s">
-        <v>23</v>
-      </c>
-      <c r="J19" s="12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="D21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" t="s">
+        <v>174</v>
+      </c>
+      <c r="F21" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" t="s">
+        <v>0</v>
+      </c>
+      <c r="H21" t="s">
+        <v>0</v>
+      </c>
+      <c r="I21" t="s">
+        <v>23</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="16">
+        <v>104</v>
+      </c>
+      <c r="B22" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" t="s">
         <v>131</v>
       </c>
-      <c r="C20" t="s">
-        <v>167</v>
-      </c>
-      <c r="D20" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" t="s">
-        <v>213</v>
-      </c>
-      <c r="F20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G20" t="s">
-        <v>0</v>
-      </c>
-      <c r="H20" t="s">
-        <v>0</v>
-      </c>
-      <c r="I20" t="s">
-        <v>23</v>
-      </c>
-      <c r="J20" s="12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="D22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" t="s">
+        <v>174</v>
+      </c>
+      <c r="F22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" t="s">
+        <v>0</v>
+      </c>
+      <c r="H22" t="s">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>23</v>
+      </c>
+      <c r="J22" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="16">
+        <v>105</v>
+      </c>
+      <c r="B23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" t="s">
         <v>132</v>
       </c>
-      <c r="C21" t="s">
-        <v>168</v>
-      </c>
-      <c r="D21" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" t="s">
-        <v>213</v>
-      </c>
-      <c r="F21" t="s">
-        <v>23</v>
-      </c>
-      <c r="G21" t="s">
-        <v>0</v>
-      </c>
-      <c r="H21" t="s">
-        <v>0</v>
-      </c>
-      <c r="I21" t="s">
-        <v>23</v>
-      </c>
-      <c r="J21" s="12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="D23" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" t="s">
+        <v>174</v>
+      </c>
+      <c r="F23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" t="s">
+        <v>0</v>
+      </c>
+      <c r="H23" t="s">
+        <v>0</v>
+      </c>
+      <c r="I23" t="s">
+        <v>23</v>
+      </c>
+      <c r="J23" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="16">
+        <v>106</v>
+      </c>
+      <c r="B24" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" t="s">
         <v>133</v>
       </c>
-      <c r="C22" t="s">
-        <v>169</v>
-      </c>
-      <c r="D22" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" t="s">
-        <v>213</v>
-      </c>
-      <c r="F22" t="s">
-        <v>23</v>
-      </c>
-      <c r="G22" t="s">
-        <v>0</v>
-      </c>
-      <c r="H22" t="s">
-        <v>0</v>
-      </c>
-      <c r="I22" t="s">
-        <v>23</v>
-      </c>
-      <c r="J22" s="12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="D24" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" t="s">
+        <v>174</v>
+      </c>
+      <c r="F24" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" t="s">
+        <v>0</v>
+      </c>
+      <c r="H24" t="s">
+        <v>0</v>
+      </c>
+      <c r="I24" t="s">
+        <v>23</v>
+      </c>
+      <c r="J24" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="16">
+        <v>107</v>
+      </c>
+      <c r="B25" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" t="s">
         <v>134</v>
       </c>
-      <c r="C23" t="s">
-        <v>170</v>
-      </c>
-      <c r="D23" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" t="s">
-        <v>213</v>
-      </c>
-      <c r="F23" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" t="s">
-        <v>0</v>
-      </c>
-      <c r="H23" t="s">
-        <v>0</v>
-      </c>
-      <c r="I23" t="s">
-        <v>23</v>
-      </c>
-      <c r="J23" s="12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="D25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" t="s">
+        <v>174</v>
+      </c>
+      <c r="F25" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" t="s">
+        <v>0</v>
+      </c>
+      <c r="H25" t="s">
+        <v>0</v>
+      </c>
+      <c r="I25" t="s">
+        <v>23</v>
+      </c>
+      <c r="J25" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="16">
+        <v>108</v>
+      </c>
+      <c r="B26" t="s">
+        <v>99</v>
+      </c>
+      <c r="C26" t="s">
         <v>135</v>
       </c>
-      <c r="C24" t="s">
-        <v>171</v>
-      </c>
-      <c r="D24" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24" t="s">
-        <v>213</v>
-      </c>
-      <c r="F24" t="s">
-        <v>23</v>
-      </c>
-      <c r="G24" t="s">
-        <v>0</v>
-      </c>
-      <c r="H24" t="s">
-        <v>0</v>
-      </c>
-      <c r="I24" t="s">
-        <v>23</v>
-      </c>
-      <c r="J24" s="12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="D26" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" t="s">
+        <v>174</v>
+      </c>
+      <c r="F26" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26" t="s">
+        <v>0</v>
+      </c>
+      <c r="I26" t="s">
+        <v>23</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="16">
+        <v>109</v>
+      </c>
+      <c r="B27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" t="s">
         <v>136</v>
       </c>
-      <c r="C25" t="s">
-        <v>172</v>
-      </c>
-      <c r="D25" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" t="s">
-        <v>213</v>
-      </c>
-      <c r="F25" t="s">
-        <v>23</v>
-      </c>
-      <c r="G25" t="s">
-        <v>0</v>
-      </c>
-      <c r="H25" t="s">
-        <v>0</v>
-      </c>
-      <c r="I25" t="s">
-        <v>23</v>
-      </c>
-      <c r="J25" s="12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="D27" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" t="s">
+        <v>174</v>
+      </c>
+      <c r="F27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" t="s">
+        <v>0</v>
+      </c>
+      <c r="H27" t="s">
+        <v>0</v>
+      </c>
+      <c r="I27" t="s">
+        <v>23</v>
+      </c>
+      <c r="J27" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="16">
+        <v>110</v>
+      </c>
+      <c r="B28" t="s">
         <v>137</v>
       </c>
-      <c r="C26" t="s">
-        <v>173</v>
-      </c>
-      <c r="D26" t="s">
-        <v>28</v>
-      </c>
-      <c r="E26" t="s">
-        <v>213</v>
-      </c>
-      <c r="F26" t="s">
-        <v>23</v>
-      </c>
-      <c r="G26" t="s">
-        <v>0</v>
-      </c>
-      <c r="H26" t="s">
-        <v>0</v>
-      </c>
-      <c r="I26" t="s">
-        <v>23</v>
-      </c>
-      <c r="J26" s="12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="C28" t="s">
         <v>138</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D28" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" t="s">
         <v>174</v>
       </c>
-      <c r="D27" t="s">
-        <v>28</v>
-      </c>
-      <c r="E27" t="s">
-        <v>213</v>
-      </c>
-      <c r="F27" t="s">
-        <v>23</v>
-      </c>
-      <c r="G27" t="s">
-        <v>0</v>
-      </c>
-      <c r="H27" t="s">
-        <v>0</v>
-      </c>
-      <c r="I27" t="s">
-        <v>23</v>
-      </c>
-      <c r="J27" s="12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="B28" t="s">
-        <v>176</v>
-      </c>
-      <c r="C28" t="s">
-        <v>177</v>
-      </c>
-      <c r="D28" t="s">
-        <v>28</v>
-      </c>
-      <c r="E28" t="s">
-        <v>213</v>
-      </c>
       <c r="F28" t="s">
         <v>23</v>
       </c>
@@ -2382,25 +2272,25 @@
       <c r="I28" t="s">
         <v>23</v>
       </c>
-      <c r="J28" s="12" t="s">
-        <v>226</v>
+      <c r="J28" s="10" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>95</v>
+      <c r="A29" s="16">
+        <v>201</v>
       </c>
       <c r="B29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" t="s">
         <v>139</v>
       </c>
-      <c r="C29" t="s">
-        <v>178</v>
-      </c>
       <c r="D29" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E29" t="s">
-        <v>213</v>
+        <v>174</v>
       </c>
       <c r="F29" t="s">
         <v>23</v>
@@ -2414,25 +2304,25 @@
       <c r="I29" t="s">
         <v>23</v>
       </c>
-      <c r="J29" s="12" t="s">
-        <v>226</v>
+      <c r="J29" s="10" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>96</v>
+      <c r="A30" s="16">
+        <v>202</v>
       </c>
       <c r="B30" t="s">
+        <v>102</v>
+      </c>
+      <c r="C30" t="s">
         <v>140</v>
       </c>
-      <c r="C30" t="s">
-        <v>179</v>
-      </c>
       <c r="D30" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E30" t="s">
-        <v>213</v>
+        <v>174</v>
       </c>
       <c r="F30" t="s">
         <v>23</v>
@@ -2446,25 +2336,25 @@
       <c r="I30" t="s">
         <v>23</v>
       </c>
-      <c r="J30" s="12" t="s">
-        <v>226</v>
+      <c r="J30" s="10" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>97</v>
+      <c r="A31" s="16">
+        <v>203</v>
       </c>
       <c r="B31" t="s">
+        <v>103</v>
+      </c>
+      <c r="C31" t="s">
         <v>141</v>
       </c>
-      <c r="C31" t="s">
-        <v>180</v>
-      </c>
       <c r="D31" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E31" t="s">
-        <v>213</v>
+        <v>174</v>
       </c>
       <c r="F31" t="s">
         <v>23</v>
@@ -2478,25 +2368,25 @@
       <c r="I31" t="s">
         <v>23</v>
       </c>
-      <c r="J31" s="12" t="s">
-        <v>226</v>
+      <c r="J31" s="10" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>98</v>
+      <c r="A32" s="16">
+        <v>204</v>
       </c>
       <c r="B32" t="s">
+        <v>104</v>
+      </c>
+      <c r="C32" t="s">
         <v>142</v>
       </c>
-      <c r="C32" t="s">
-        <v>181</v>
-      </c>
       <c r="D32" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E32" t="s">
-        <v>213</v>
+        <v>174</v>
       </c>
       <c r="F32" t="s">
         <v>23</v>
@@ -2510,25 +2400,25 @@
       <c r="I32" t="s">
         <v>23</v>
       </c>
-      <c r="J32" s="12" t="s">
-        <v>226</v>
+      <c r="J32" s="10" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>99</v>
+      <c r="A33" s="16">
+        <v>205</v>
       </c>
       <c r="B33" t="s">
+        <v>105</v>
+      </c>
+      <c r="C33" t="s">
         <v>143</v>
       </c>
-      <c r="C33" t="s">
-        <v>182</v>
-      </c>
       <c r="D33" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E33" t="s">
-        <v>213</v>
+        <v>174</v>
       </c>
       <c r="F33" t="s">
         <v>23</v>
@@ -2542,25 +2432,25 @@
       <c r="I33" t="s">
         <v>23</v>
       </c>
-      <c r="J33" s="12" t="s">
-        <v>226</v>
+      <c r="J33" s="10" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>100</v>
+      <c r="A34" s="16">
+        <v>206</v>
       </c>
       <c r="B34" t="s">
+        <v>106</v>
+      </c>
+      <c r="C34" t="s">
         <v>144</v>
       </c>
-      <c r="C34" t="s">
-        <v>183</v>
-      </c>
       <c r="D34" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E34" t="s">
-        <v>213</v>
+        <v>174</v>
       </c>
       <c r="F34" t="s">
         <v>23</v>
@@ -2574,25 +2464,25 @@
       <c r="I34" t="s">
         <v>23</v>
       </c>
-      <c r="J34" s="12" t="s">
-        <v>226</v>
+      <c r="J34" s="10" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>101</v>
+      <c r="A35" s="16">
+        <v>207</v>
       </c>
       <c r="B35" t="s">
+        <v>107</v>
+      </c>
+      <c r="C35" t="s">
         <v>145</v>
       </c>
-      <c r="C35" t="s">
-        <v>184</v>
-      </c>
       <c r="D35" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E35" t="s">
-        <v>213</v>
+        <v>174</v>
       </c>
       <c r="F35" t="s">
         <v>23</v>
@@ -2606,25 +2496,25 @@
       <c r="I35" t="s">
         <v>23</v>
       </c>
-      <c r="J35" s="12" t="s">
-        <v>226</v>
+      <c r="J35" s="10" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>102</v>
+      <c r="A36" s="16">
+        <v>208</v>
       </c>
       <c r="B36" t="s">
+        <v>108</v>
+      </c>
+      <c r="C36" t="s">
         <v>146</v>
       </c>
-      <c r="C36" t="s">
-        <v>185</v>
-      </c>
       <c r="D36" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E36" t="s">
-        <v>213</v>
+        <v>174</v>
       </c>
       <c r="F36" t="s">
         <v>23</v>
@@ -2638,25 +2528,25 @@
       <c r="I36" t="s">
         <v>23</v>
       </c>
-      <c r="J36" s="12" t="s">
-        <v>226</v>
+      <c r="J36" s="10" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>103</v>
+      <c r="A37" s="16">
+        <v>209</v>
       </c>
       <c r="B37" t="s">
+        <v>109</v>
+      </c>
+      <c r="C37" t="s">
         <v>147</v>
       </c>
-      <c r="C37" t="s">
-        <v>186</v>
-      </c>
       <c r="D37" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E37" t="s">
-        <v>213</v>
+        <v>174</v>
       </c>
       <c r="F37" t="s">
         <v>23</v>
@@ -2670,57 +2560,57 @@
       <c r="I37" t="s">
         <v>23</v>
       </c>
-      <c r="J37" s="12" t="s">
-        <v>226</v>
+      <c r="J37" s="10" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>104</v>
+      <c r="A38" s="16">
+        <v>210</v>
       </c>
       <c r="B38" t="s">
+        <v>110</v>
+      </c>
+      <c r="C38" t="s">
         <v>148</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
+        <v>25</v>
+      </c>
+      <c r="E38" t="s">
+        <v>174</v>
+      </c>
+      <c r="F38" t="s">
+        <v>23</v>
+      </c>
+      <c r="G38" t="s">
+        <v>0</v>
+      </c>
+      <c r="H38" t="s">
+        <v>0</v>
+      </c>
+      <c r="I38" t="s">
+        <v>23</v>
+      </c>
+      <c r="J38" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="D38" t="s">
-        <v>28</v>
-      </c>
-      <c r="E38" t="s">
-        <v>213</v>
-      </c>
-      <c r="F38" t="s">
-        <v>23</v>
-      </c>
-      <c r="G38" t="s">
-        <v>0</v>
-      </c>
-      <c r="H38" t="s">
-        <v>0</v>
-      </c>
-      <c r="I38" t="s">
-        <v>23</v>
-      </c>
-      <c r="J38" s="12" t="s">
-        <v>226</v>
-      </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>108</v>
+      <c r="A39" s="16">
+        <v>211</v>
       </c>
       <c r="B39" t="s">
+        <v>111</v>
+      </c>
+      <c r="C39" t="s">
         <v>149</v>
       </c>
-      <c r="C39" t="s">
-        <v>188</v>
-      </c>
       <c r="D39" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E39" t="s">
-        <v>213</v>
+        <v>174</v>
       </c>
       <c r="F39" t="s">
         <v>23</v>
@@ -2734,25 +2624,25 @@
       <c r="I39" t="s">
         <v>23</v>
       </c>
-      <c r="J39" s="12" t="s">
-        <v>226</v>
+      <c r="J39" s="10" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>109</v>
+      <c r="A40" s="16">
+        <v>212</v>
       </c>
       <c r="B40" t="s">
+        <v>112</v>
+      </c>
+      <c r="C40" t="s">
         <v>150</v>
       </c>
-      <c r="C40" t="s">
-        <v>189</v>
-      </c>
       <c r="D40" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E40" t="s">
-        <v>213</v>
+        <v>174</v>
       </c>
       <c r="F40" t="s">
         <v>23</v>
@@ -2766,8 +2656,8 @@
       <c r="I40" t="s">
         <v>23</v>
       </c>
-      <c r="J40" s="12" t="s">
-        <v>226</v>
+      <c r="J40" s="10" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2776,26 +2666,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="N1" sqref="N1"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="16" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" style="16" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="23" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19.28515625" bestFit="1" customWidth="1"/>
@@ -2808,58 +2698,58 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="I1" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="K1" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="L1" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="N1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="Q1" s="3" t="s">
-        <v>235</v>
+        <v>194</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>221</v>
+        <v>182</v>
       </c>
       <c r="S1" s="3" t="s">
         <v>4</v>
@@ -2867,21 +2757,21 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>218</v>
+        <v>179</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>179</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="14" t="s">
         <v>16</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -2890,13 +2780,13 @@
       <c r="H2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="K2" s="3" t="s">
+      <c r="I2" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="14" t="s">
         <v>20</v>
       </c>
       <c r="L2" s="3" t="s">
@@ -2931,16 +2821,16 @@
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="14" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="E3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>0</v>
       </c>
       <c r="G3" s="3" t="s">
@@ -2949,13 +2839,13 @@
       <c r="H3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="3" t="s">
+      <c r="I3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="14" t="s">
         <v>0</v>
       </c>
       <c r="L3" s="3" t="s">
@@ -2985,35 +2875,35 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>219</v>
+        <v>180</v>
       </c>
       <c r="C4" t="s">
-        <v>236</v>
+        <v>195</v>
       </c>
       <c r="D4"/>
-      <c r="E4" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G4" s="6">
+      <c r="E4" s="16">
+        <v>10</v>
+      </c>
+      <c r="G4" s="5">
         <v>40543</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>40543</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="K4" t="s">
-        <v>83</v>
+      <c r="I4" s="15">
+        <v>2010</v>
+      </c>
+      <c r="J4" s="15">
+        <v>2010</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>68</v>
       </c>
       <c r="L4" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="M4" t="s">
         <v>23</v>
@@ -3022,10 +2912,10 @@
         <v>0</v>
       </c>
       <c r="O4" t="s">
-        <v>243</v>
+        <v>202</v>
       </c>
       <c r="P4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="Q4" t="s">
         <v>23</v>
@@ -3034,40 +2924,40 @@
         <v>24</v>
       </c>
       <c r="S4" t="s">
-        <v>225</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>223</v>
+        <v>184</v>
       </c>
       <c r="B5" t="s">
-        <v>224</v>
+        <v>185</v>
       </c>
       <c r="C5" t="s">
-        <v>237</v>
+        <v>196</v>
       </c>
       <c r="D5"/>
-      <c r="E5" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G5" s="6">
+      <c r="E5" s="16">
+        <v>10</v>
+      </c>
+      <c r="G5" s="5">
         <v>40543</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <v>40543</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="K5" t="s">
-        <v>83</v>
+      <c r="I5" s="15">
+        <v>2010</v>
+      </c>
+      <c r="J5" s="15">
+        <v>2010</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>68</v>
       </c>
       <c r="L5" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="M5" t="s">
         <v>23</v>
@@ -3076,10 +2966,10 @@
         <v>0</v>
       </c>
       <c r="O5" t="s">
-        <v>243</v>
+        <v>202</v>
       </c>
       <c r="P5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="Q5" t="s">
         <v>23</v>
@@ -3088,7 +2978,7 @@
         <v>24</v>
       </c>
       <c r="S5" t="s">
-        <v>225</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -3098,18 +2988,18 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:W8"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T3" sqref="T3"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.7109375" style="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
@@ -3124,100 +3014,100 @@
     <col min="15" max="15" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.85546875" style="16" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="33.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="H1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>238</v>
+        <v>197</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>239</v>
+        <v>198</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>43</v>
+        <v>199</v>
+      </c>
+      <c r="R1" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="S1" s="14" t="s">
+        <v>38</v>
       </c>
       <c r="T1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="17" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>1</v>
@@ -3235,7 +3125,7 @@
         <v>21</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>241</v>
+        <v>200</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>1</v>
@@ -3243,24 +3133,24 @@
       <c r="Q2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="R2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>49</v>
+      <c r="R2" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="S2" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="T2" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -3305,28 +3195,28 @@
       <c r="Q3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="R3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="S3" s="3" t="s">
+      <c r="R3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="S3" s="14" t="s">
         <v>0</v>
       </c>
       <c r="T3" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>104</v>
+        <v>67</v>
+      </c>
+      <c r="B4" s="16">
+        <v>2010</v>
+      </c>
+      <c r="C4" s="16">
+        <v>210</v>
       </c>
       <c r="D4" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="E4">
         <v>1.72</v>
@@ -3343,50 +3233,57 @@
       <c r="I4">
         <v>85.86</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="5">
         <v>40179</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="5">
         <v>40179</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="5">
         <v>40543</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="5">
         <v>40543</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="P4" s="6">
+        <v>203</v>
+      </c>
+      <c r="P4" s="5">
         <v>40179</v>
       </c>
-      <c r="Q4" s="6">
+      <c r="Q4" s="5">
         <v>40179</v>
       </c>
-      <c r="R4" s="6"/>
-      <c r="S4" s="4" t="s">
-        <v>82</v>
+      <c r="S4" s="16">
+        <v>2010</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.45">
+        <v>186</v>
+      </c>
+      <c r="V4">
+        <f>_xlfn.NUMBERVALUE(B4)</f>
+        <v>2010</v>
+      </c>
+      <c r="W4">
+        <f>_xlfn.NUMBERVALUE(C4)</f>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>108</v>
+        <v>67</v>
+      </c>
+      <c r="B5" s="16">
+        <v>2011</v>
+      </c>
+      <c r="C5" s="16">
+        <v>211</v>
       </c>
       <c r="D5" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="E5">
         <v>17.97</v>
@@ -3403,50 +3300,57 @@
       <c r="I5">
         <v>35.61</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="5">
         <v>40179</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="5">
         <v>40179</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="5">
         <v>40543</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="5">
         <v>40543</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="P5" s="6">
+        <v>204</v>
+      </c>
+      <c r="P5" s="5">
         <v>40179</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="Q5" s="5">
         <v>40179</v>
       </c>
-      <c r="R5" s="6"/>
-      <c r="S5" s="4" t="s">
-        <v>82</v>
+      <c r="S5" s="16">
+        <v>2010</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.45">
+        <v>186</v>
+      </c>
+      <c r="V5">
+        <f t="shared" ref="V5:V8" si="0">_xlfn.NUMBERVALUE(B5)</f>
+        <v>2011</v>
+      </c>
+      <c r="W5">
+        <f t="shared" ref="W5:W8" si="1">_xlfn.NUMBERVALUE(C5)</f>
+        <v>211</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>109</v>
+        <v>67</v>
+      </c>
+      <c r="B6" s="16">
+        <v>2012</v>
+      </c>
+      <c r="C6" s="16">
+        <v>212</v>
       </c>
       <c r="D6" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="E6">
         <v>1.72</v>
@@ -3463,50 +3367,57 @@
       <c r="I6">
         <v>85.86</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <v>40179</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="5">
         <v>40179</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="5">
         <v>40543</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="5">
         <v>40543</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="P6" s="6">
+        <v>203</v>
+      </c>
+      <c r="P6" s="5">
         <v>40179</v>
       </c>
-      <c r="Q6" s="6">
+      <c r="Q6" s="5">
         <v>40179</v>
       </c>
-      <c r="R6" s="6"/>
-      <c r="S6" s="4" t="s">
-        <v>82</v>
+      <c r="S6" s="16">
+        <v>2010</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.45">
+        <v>186</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="0"/>
+        <v>2012</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="1"/>
+        <v>212</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>223</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>104</v>
+        <v>184</v>
+      </c>
+      <c r="B7" s="16">
+        <v>2013</v>
+      </c>
+      <c r="C7" s="16">
+        <v>210</v>
       </c>
       <c r="D7" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="E7">
         <v>17.97</v>
@@ -3523,50 +3434,57 @@
       <c r="I7">
         <v>35.61</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="5">
         <v>40179</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="5">
         <v>40179</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="5">
         <v>40543</v>
       </c>
-      <c r="M7" s="6">
+      <c r="M7" s="5">
         <v>40543</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="P7" s="6">
+        <v>204</v>
+      </c>
+      <c r="P7" s="5">
         <v>40179</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="Q7" s="5">
         <v>40179</v>
       </c>
-      <c r="R7" s="6"/>
-      <c r="S7" s="4" t="s">
-        <v>82</v>
+      <c r="S7" s="16">
+        <v>2010</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.45">
+        <v>186</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="0"/>
+        <v>2013</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="1"/>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>223</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>108</v>
+        <v>184</v>
+      </c>
+      <c r="B8" s="16">
+        <v>2014</v>
+      </c>
+      <c r="C8" s="16">
+        <v>211</v>
       </c>
       <c r="D8" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="E8">
         <v>1.72</v>
@@ -3583,36 +3501,43 @@
       <c r="I8">
         <v>85.86</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="5">
         <v>40179</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="5">
         <v>40179</v>
       </c>
-      <c r="L8" s="6">
+      <c r="L8" s="5">
         <v>40543</v>
       </c>
-      <c r="M8" s="6">
+      <c r="M8" s="5">
         <v>40543</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="P8" s="6">
+        <v>203</v>
+      </c>
+      <c r="P8" s="5">
         <v>40179</v>
       </c>
-      <c r="Q8" s="6">
+      <c r="Q8" s="5">
         <v>40179</v>
       </c>
-      <c r="R8" s="6"/>
-      <c r="S8" s="4" t="s">
-        <v>82</v>
+      <c r="S8" s="16">
+        <v>2010</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>225</v>
+        <v>186</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="0"/>
+        <v>2014</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="1"/>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -3621,56 +3546,56 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>65</v>
+      <c r="A1" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>60</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="14" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -3681,45 +3606,45 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>106</v>
+      <c r="A4" s="16">
+        <v>2010</v>
+      </c>
+      <c r="B4" s="16">
+        <v>2011</v>
       </c>
       <c r="C4" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>225</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A5" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>107</v>
+      <c r="A5" s="16">
+        <v>2010</v>
+      </c>
+      <c r="B5" s="16">
+        <v>2012</v>
       </c>
       <c r="C5" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>225</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>228</v>
+      <c r="A6" s="16">
+        <v>2013</v>
+      </c>
+      <c r="B6" s="16">
+        <v>2014</v>
       </c>
       <c r="C6" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>225</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -3728,7 +3653,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3747,16 +3672,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>4</v>
@@ -3764,7 +3689,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>22</v>
@@ -3773,7 +3698,7 @@
         <v>22</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>19</v>
@@ -3798,19 +3723,19 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>223</v>
+        <v>184</v>
       </c>
       <c r="B4" t="s">
-        <v>222</v>
+        <v>183</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D4">
         <v>0.5</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>225</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -3819,7 +3744,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3838,13 +3763,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>242</v>
+        <v>201</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>4</v>
@@ -3852,13 +3777,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>19</v>
@@ -3880,44 +3805,44 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>73</v>
       </c>
       <c r="C4">
         <v>100</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>225</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>223</v>
+        <v>184</v>
       </c>
       <c r="B5" t="s">
-        <v>110</v>
+        <v>72</v>
       </c>
       <c r="C5">
         <v>25</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>225</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>223</v>
+        <v>184</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>74</v>
       </c>
       <c r="C6">
         <v>75</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>225</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -3926,10 +3851,10 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
@@ -3946,96 +3871,96 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>190</v>
+        <v>151</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>191</v>
+        <v>152</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>192</v>
+        <v>153</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>193</v>
+        <v>154</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>194</v>
+        <v>155</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>195</v>
+        <v>156</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>196</v>
+        <v>157</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>197</v>
+        <v>158</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>198</v>
+        <v>159</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>199</v>
+        <v>160</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>200</v>
+        <v>161</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>201</v>
+        <v>162</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>202</v>
+        <v>163</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>203</v>
+        <v>164</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>204</v>
+        <v>165</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>205</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>113</v>
+        <v>75</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>21</v>

</xml_diff>